<commit_message>
formatting for metrics table
</commit_message>
<xml_diff>
--- a/data/metrics/metrics_table.xlsx
+++ b/data/metrics/metrics_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keith\code\StrategyDocumentAnalysis\data\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D246A48-FCB0-4B33-ABB5-D4A148C7227B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7016308B-4401-4F5C-B3F4-C01DDAF60A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="29829" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -302,35 +302,35 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Bierstadt"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Bierstadt"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Bierstadt"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Bierstadt"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Bierstadt"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -508,6 +508,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -882,7 +888,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -926,9 +932,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="18" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -937,16 +961,31 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="4" borderId="20" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="2" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="2" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="20" fillId="3" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -955,79 +994,118 @@
     </xf>
     <xf numFmtId="164" fontId="20" fillId="3" borderId="20" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="4" borderId="10" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="22" fillId="2" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="2" borderId="14" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="2" borderId="13" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="4" borderId="14" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="4" borderId="13" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="13" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="14" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="13" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="10" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="15" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="4" borderId="21" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="22" fillId="2" borderId="21" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="2" borderId="16" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="22" fillId="2" borderId="15" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="21" fillId="4" borderId="15" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="21" fillId="4" borderId="16" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="20" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="21" fillId="4" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="20" fillId="3" borderId="15" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="4" borderId="21" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="2" borderId="21" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="2" borderId="16" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="2" borderId="15" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="19" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="22" fillId="2" borderId="15" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="21" fillId="4" borderId="21" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="20" fillId="3" borderId="17" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="4" borderId="19" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="19" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="22" fillId="2" borderId="19" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="2" borderId="18" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="22" fillId="2" borderId="17" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1037,36 +1115,54 @@
     <xf numFmtId="2" fontId="21" fillId="4" borderId="17" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="21" fillId="4" borderId="19" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="20" fillId="3" borderId="14" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="20" fillId="3" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="4" borderId="10" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="2" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="2" borderId="14" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="21" fillId="4" borderId="14" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="21" fillId="4" borderId="13" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="21" fillId="4" borderId="10" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="20" fillId="3" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="20" fillId="3" borderId="14" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="20" fillId="3" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="4" borderId="10" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="22" fillId="2" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="2" borderId="14" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="22" fillId="2" borderId="13" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1076,103 +1172,20 @@
     <xf numFmtId="2" fontId="21" fillId="4" borderId="13" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="21" fillId="4" borderId="10" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="20" fillId="3" borderId="14" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="20" fillId="3" borderId="15" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="20" fillId="3" borderId="21" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="14" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="15" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="21" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="21" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="15" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="22" fillId="2" borderId="21" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="22" fillId="2" borderId="16" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="3" borderId="17" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="2" borderId="19" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="2" borderId="18" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="3" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="22" fillId="2" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="22" fillId="2" borderId="14" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="3" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="2" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="2" borderId="14" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2045,10 +2058,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:N17"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2056,475 +2069,531 @@
     <col min="1" max="1" width="2.84375" customWidth="1"/>
     <col min="2" max="2" width="11.765625" customWidth="1"/>
     <col min="3" max="3" width="18.4609375" style="14" customWidth="1"/>
-    <col min="4" max="14" width="6.23046875" style="1" customWidth="1"/>
+    <col min="4" max="8" width="6.23046875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="7.15234375" style="1" customWidth="1"/>
+    <col min="11" max="14" width="6.23046875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B2" s="72" t="s">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="98"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
+      <c r="N1" s="100"/>
+      <c r="O1" s="98"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A2" s="98"/>
+      <c r="B2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="72" t="s">
+      <c r="D2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="72" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="74"/>
-      <c r="K2" s="72" t="s">
+      <c r="J2" s="18"/>
+      <c r="K2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="74"/>
-    </row>
-    <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="77"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="15" t="s">
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="98"/>
+    </row>
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="98"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="22">
         <v>0.25</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="22">
         <v>0.5</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="22">
         <v>0.75</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="L3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="M3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="2:14" ht="28.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="69" t="s">
+      <c r="O3" s="98"/>
+    </row>
+    <row r="4" spans="1:15" ht="28.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="98"/>
+      <c r="B4" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="78">
+      <c r="D4" s="27">
         <v>7</v>
       </c>
-      <c r="E4" s="40">
+      <c r="E4" s="28">
         <v>8.375</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="29">
         <v>9</v>
       </c>
-      <c r="G4" s="79">
+      <c r="G4" s="30">
         <v>10</v>
       </c>
-      <c r="H4" s="39">
+      <c r="H4" s="31">
         <v>11.5</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="32">
         <v>9</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="33">
         <v>6.5</v>
       </c>
-      <c r="K4" s="23">
+      <c r="K4" s="34">
         <v>8</v>
       </c>
-      <c r="L4" s="24">
+      <c r="L4" s="35">
         <v>6</v>
       </c>
-      <c r="M4" s="24">
+      <c r="M4" s="35">
         <v>4</v>
       </c>
-      <c r="N4" s="22">
+      <c r="N4" s="33">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="5" spans="2:14" ht="28.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="71"/>
-      <c r="C5" s="25" t="s">
+      <c r="O4" s="98"/>
+    </row>
+    <row r="5" spans="1:15" ht="28.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="98"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="80">
+      <c r="D5" s="38">
         <v>3.65</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="39">
         <v>7.125</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="40">
         <v>8.3849999999999998</v>
       </c>
-      <c r="G5" s="81">
+      <c r="G5" s="41">
         <v>8.83</v>
       </c>
-      <c r="H5" s="82">
+      <c r="H5" s="42">
         <v>9.27</v>
       </c>
-      <c r="I5" s="28">
+      <c r="I5" s="43">
         <v>9.18</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="44">
         <v>5.15</v>
       </c>
-      <c r="K5" s="30">
+      <c r="K5" s="45">
         <v>6.63</v>
       </c>
-      <c r="L5" s="31">
+      <c r="L5" s="39">
         <v>5.67</v>
       </c>
-      <c r="M5" s="32">
+      <c r="M5" s="46">
         <v>3.08</v>
       </c>
-      <c r="N5" s="27" t="s">
+      <c r="N5" s="47" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="2:14" ht="28.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="70"/>
-      <c r="C6" s="33" t="s">
+      <c r="O5" s="98"/>
+    </row>
+    <row r="6" spans="1:15" ht="28.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="98"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="83">
+      <c r="D6" s="50">
         <v>34.51</v>
       </c>
-      <c r="E6" s="84">
+      <c r="E6" s="51">
         <v>62.37</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="52">
         <v>68.41</v>
       </c>
-      <c r="G6" s="85">
+      <c r="G6" s="53">
         <v>74.790000000000006</v>
       </c>
-      <c r="H6" s="36">
+      <c r="H6" s="54">
         <v>85.72</v>
       </c>
-      <c r="I6" s="86">
+      <c r="I6" s="55">
         <v>75.290000000000006</v>
       </c>
-      <c r="J6" s="36">
+      <c r="J6" s="54">
         <v>84.12</v>
       </c>
-      <c r="K6" s="37">
+      <c r="K6" s="56">
         <v>60.89</v>
       </c>
-      <c r="L6" s="34">
+      <c r="L6" s="52">
         <v>67.37</v>
       </c>
-      <c r="M6" s="34">
+      <c r="M6" s="52">
         <v>64.63</v>
       </c>
-      <c r="N6" s="38">
+      <c r="N6" s="57">
         <v>53.96</v>
       </c>
-    </row>
-    <row r="7" spans="2:14" ht="28.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="69" t="s">
+      <c r="O6" s="98"/>
+    </row>
+    <row r="7" spans="1:15" ht="28.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="98"/>
+      <c r="B7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="78">
+      <c r="D7" s="27">
         <v>16.899999999999999</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="28">
         <v>22.1</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="29">
         <v>29.55</v>
       </c>
-      <c r="G7" s="79">
+      <c r="G7" s="30">
         <v>35.674999999999997</v>
       </c>
-      <c r="H7" s="39">
+      <c r="H7" s="31">
         <v>100</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="32">
         <v>30.9</v>
       </c>
-      <c r="J7" s="39">
+      <c r="J7" s="31">
         <v>49.7</v>
       </c>
-      <c r="K7" s="23">
+      <c r="K7" s="34">
         <v>18.2</v>
       </c>
-      <c r="L7" s="40">
+      <c r="L7" s="28">
         <v>19.600000000000001</v>
       </c>
-      <c r="M7" s="21" t="s">
+      <c r="M7" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="N7" s="41">
+      <c r="N7" s="58">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="2:14" ht="28.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="70"/>
-      <c r="C8" s="33" t="s">
+      <c r="O7" s="98"/>
+    </row>
+    <row r="8" spans="1:15" ht="28.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="98"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="67">
+      <c r="D8" s="59">
         <v>6.52</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="60">
         <v>63.075000000000003</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F8" s="61">
         <v>187.31</v>
       </c>
-      <c r="G8" s="87">
+      <c r="G8" s="62">
         <v>421.05499999999898</v>
       </c>
-      <c r="H8" s="88">
+      <c r="H8" s="63">
         <v>3638.78</v>
       </c>
-      <c r="I8" s="45">
+      <c r="I8" s="64">
         <v>514.70000000000005</v>
       </c>
-      <c r="J8" s="44">
+      <c r="J8" s="65">
         <v>242.78</v>
       </c>
-      <c r="K8" s="42">
+      <c r="K8" s="66">
         <v>108.88</v>
       </c>
-      <c r="L8" s="43">
+      <c r="L8" s="61">
         <v>181.32</v>
       </c>
-      <c r="M8" s="46">
+      <c r="M8" s="60">
         <v>47.53</v>
       </c>
-      <c r="N8" s="44">
+      <c r="N8" s="65">
         <v>135.78</v>
       </c>
-    </row>
-    <row r="9" spans="2:14" ht="28.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="69" t="s">
+      <c r="O8" s="98"/>
+    </row>
+    <row r="9" spans="1:15" ht="28.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="98"/>
+      <c r="B9" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="89">
+      <c r="D9" s="68">
         <v>0.38136489000000001</v>
       </c>
-      <c r="E9" s="52">
+      <c r="E9" s="69">
         <v>0.68396257275000005</v>
       </c>
-      <c r="F9" s="48">
+      <c r="F9" s="70">
         <v>0.77435306549999905</v>
       </c>
-      <c r="G9" s="90">
+      <c r="G9" s="71">
         <v>0.81104396050000005</v>
       </c>
-      <c r="H9" s="91">
+      <c r="H9" s="72">
         <v>0.87307593100000003</v>
       </c>
-      <c r="I9" s="49">
+      <c r="I9" s="73">
         <v>0.86390302600000002</v>
       </c>
-      <c r="J9" s="50">
+      <c r="J9" s="74">
         <v>0.53745041999999998</v>
       </c>
-      <c r="K9" s="51">
+      <c r="K9" s="75">
         <v>0.46246300899999998</v>
       </c>
-      <c r="L9" s="52">
+      <c r="L9" s="69">
         <v>0.51978007000000004</v>
       </c>
-      <c r="M9" s="52">
+      <c r="M9" s="69">
         <v>0.55558583299999997</v>
       </c>
-      <c r="N9" s="50">
+      <c r="N9" s="74">
         <v>0.49386511399999999</v>
       </c>
-    </row>
-    <row r="10" spans="2:14" ht="28.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="71"/>
-      <c r="C10" s="25" t="s">
+      <c r="O9" s="98"/>
+    </row>
+    <row r="10" spans="1:15" ht="28.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="98"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="80">
+      <c r="D10" s="38">
         <v>4.4800000000000004</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="39">
         <v>6.9275000000000002</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="40">
         <v>7.88</v>
       </c>
-      <c r="G10" s="81">
+      <c r="G10" s="41">
         <v>8.6374999999999993</v>
       </c>
-      <c r="H10" s="82">
+      <c r="H10" s="42">
         <v>9.26</v>
       </c>
-      <c r="I10" s="28">
+      <c r="I10" s="43">
         <v>8.9600000000000009</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="44">
         <v>6.03</v>
       </c>
-      <c r="K10" s="30">
+      <c r="K10" s="45">
         <v>6.3</v>
       </c>
-      <c r="L10" s="26">
+      <c r="L10" s="40">
         <v>7.19</v>
       </c>
-      <c r="M10" s="31">
+      <c r="M10" s="39">
         <v>6.04</v>
       </c>
-      <c r="N10" s="53">
+      <c r="N10" s="76">
         <v>2.94</v>
       </c>
-    </row>
-    <row r="11" spans="2:14" ht="28.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="71"/>
-      <c r="C11" s="25" t="s">
+      <c r="O10" s="98"/>
+    </row>
+    <row r="11" spans="1:15" ht="28.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="98"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="92">
+      <c r="D11" s="77">
         <v>32</v>
       </c>
-      <c r="E11" s="58">
+      <c r="E11" s="78">
         <v>78</v>
       </c>
-      <c r="F11" s="55">
+      <c r="F11" s="79">
         <v>90</v>
       </c>
-      <c r="G11" s="93">
+      <c r="G11" s="80">
         <v>96</v>
       </c>
-      <c r="H11" s="94">
+      <c r="H11" s="81">
         <v>100</v>
       </c>
-      <c r="I11" s="54">
+      <c r="I11" s="82">
         <v>95</v>
       </c>
-      <c r="J11" s="56">
+      <c r="J11" s="83">
         <v>47</v>
       </c>
-      <c r="K11" s="57">
+      <c r="K11" s="84">
         <v>58</v>
       </c>
-      <c r="L11" s="58">
+      <c r="L11" s="78">
         <v>53</v>
       </c>
-      <c r="M11" s="59">
+      <c r="M11" s="85">
         <v>30</v>
       </c>
-      <c r="N11" s="60">
+      <c r="N11" s="86">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="2:14" ht="28.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="71"/>
-      <c r="C12" s="25" t="s">
+      <c r="O11" s="98"/>
+    </row>
+    <row r="12" spans="1:15" ht="28.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="98"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="95">
+      <c r="D12" s="87">
         <v>0.11799999999999999</v>
       </c>
-      <c r="E12" s="65">
+      <c r="E12" s="88">
         <v>0.5595</v>
       </c>
-      <c r="F12" s="61">
+      <c r="F12" s="89">
         <v>0.74</v>
       </c>
-      <c r="G12" s="96">
+      <c r="G12" s="90">
         <v>0.80225000000000002</v>
       </c>
-      <c r="H12" s="97">
+      <c r="H12" s="91">
         <v>0.88900000000000001</v>
       </c>
-      <c r="I12" s="62">
+      <c r="I12" s="92">
         <v>0.81399999999999995</v>
       </c>
-      <c r="J12" s="63">
+      <c r="J12" s="93">
         <v>0.33900000000000002</v>
       </c>
-      <c r="K12" s="64">
+      <c r="K12" s="94">
         <v>0.42199999999999999</v>
       </c>
-      <c r="L12" s="65">
+      <c r="L12" s="88">
         <v>0.30399999999999999</v>
       </c>
-      <c r="M12" s="65">
+      <c r="M12" s="88">
         <v>0.17899999999999999</v>
       </c>
-      <c r="N12" s="66">
+      <c r="N12" s="95">
         <v>0.115</v>
       </c>
-    </row>
-    <row r="13" spans="2:14" ht="28.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="70"/>
-      <c r="C13" s="33" t="s">
+      <c r="O12" s="98"/>
+    </row>
+    <row r="13" spans="1:15" ht="28.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="98"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="67">
+      <c r="D13" s="59">
         <v>33.5</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="60">
         <v>49</v>
       </c>
-      <c r="F13" s="43">
+      <c r="F13" s="61">
         <v>53.5</v>
       </c>
-      <c r="G13" s="87">
+      <c r="G13" s="62">
         <v>65</v>
       </c>
-      <c r="H13" s="88">
+      <c r="H13" s="63">
         <v>73</v>
       </c>
-      <c r="I13" s="45">
+      <c r="I13" s="64">
         <v>79</v>
       </c>
-      <c r="J13" s="44">
+      <c r="J13" s="65">
         <v>60</v>
       </c>
-      <c r="K13" s="67">
+      <c r="K13" s="59">
         <v>25</v>
       </c>
-      <c r="L13" s="68">
+      <c r="L13" s="96">
         <v>10</v>
       </c>
-      <c r="M13" s="46">
+      <c r="M13" s="60">
         <v>34</v>
       </c>
-      <c r="N13" s="35" t="s">
+      <c r="N13" s="97" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B14" s="14"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="O13" s="98"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A14" s="98"/>
+      <c r="B14" s="99"/>
+      <c r="C14" s="99"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="100"/>
+      <c r="F14" s="100"/>
+      <c r="G14" s="100"/>
+      <c r="H14" s="100"/>
+      <c r="I14" s="100"/>
+      <c r="J14" s="100"/>
+      <c r="K14" s="100"/>
+      <c r="L14" s="100"/>
+      <c r="M14" s="100"/>
+      <c r="N14" s="100"/>
+      <c r="O14" s="98"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B15" s="14"/>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B16" s="14"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.4">

</xml_diff>